<commit_message>
new look begining @mac
</commit_message>
<xml_diff>
--- a/GFDRR Trustee Names.xlsx
+++ b/GFDRR Trustee Names.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WB523713\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresgf91/World_Bank/GFDRR/Shiny_Dashboards/Github_Code/GFDRR_Grant-Monitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{66C387E1-36EE-4F8B-A3E3-ED98AE9C3685}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D5734C-D9D6-4045-85FE-245553002BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E8C3BC2D-A0E5-480E-893C-5B94551D54C0}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{E8C3BC2D-A0E5-480E-893C-5B94551D54C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Trustee</t>
   </si>
@@ -145,6 +145,12 @@
   </si>
   <si>
     <t>ACP-EU NDRR</t>
+  </si>
+  <si>
+    <t>TF070808</t>
+  </si>
+  <si>
+    <t>Sweden Non-Core TF</t>
   </si>
 </sst>
 </file>
@@ -518,18 +524,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88F7D9B-B81B-494F-860C-D51A2EA83D26}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -537,7 +543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -545,7 +551,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -553,7 +559,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -561,7 +567,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -569,7 +575,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -577,7 +583,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
@@ -585,7 +591,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -593,7 +599,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
@@ -601,7 +607,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -609,7 +615,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -617,7 +623,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
@@ -625,7 +631,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>13</v>
       </c>
@@ -633,7 +639,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
@@ -641,7 +647,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
@@ -649,7 +655,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>16</v>
       </c>
@@ -657,7 +663,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -665,7 +671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>18</v>
       </c>
@@ -673,12 +679,20 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -687,6 +701,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F9144FF4F5C63446B197BD2423D4BE63" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3374a5aae0a160fa8f7d756ba445b37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3ab36575-1774-42a5-8ba0-d07685207d4a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4a19d2d0fdc8380b0ce6c7c07b928d91" ns2:_="">
     <xsd:import namespace="3ab36575-1774-42a5-8ba0-d07685207d4a"/>
@@ -818,15 +841,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -834,13 +848,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8092C04-3B86-48C3-AACA-8E92DC3775F3}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B3E7EE6-44C7-4FC4-8FBC-FB4EDCF13A75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B3E7EE6-44C7-4FC4-8FBC-FB4EDCF13A75}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8092C04-3B86-48C3-AACA-8E92DC3775F3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3ab36575-1774-42a5-8ba0-d07685207d4a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF067616-7EC9-46F6-A8EA-7CB68C3B6A9D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF067616-7EC9-46F6-A8EA-7CB68C3B6A9D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
reports and UX @ mac
</commit_message>
<xml_diff>
--- a/GFDRR Trustee Names.xlsx
+++ b/GFDRR Trustee Names.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andresgf91/World_Bank/GFDRR/Shiny_Dashboards/Github_Code/GFDRR_Grant-Monitoring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D5734C-D9D6-4045-85FE-245553002BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD436C69-15B3-EB40-BE6B-9239F8A74F41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15840" xr2:uid="{E8C3BC2D-A0E5-480E-893C-5B94551D54C0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Trustee</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Sweden Non-Core TF</t>
+  </si>
+  <si>
+    <t>TF073410</t>
+  </si>
+  <si>
+    <t>Core MDTF II</t>
   </si>
 </sst>
 </file>
@@ -524,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88F7D9B-B81B-494F-860C-D51A2EA83D26}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -695,21 +701,20 @@
         <v>39</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F9144FF4F5C63446B197BD2423D4BE63" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d3374a5aae0a160fa8f7d756ba445b37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3ab36575-1774-42a5-8ba0-d07685207d4a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4a19d2d0fdc8380b0ce6c7c07b928d91" ns2:_="">
     <xsd:import namespace="3ab36575-1774-42a5-8ba0-d07685207d4a"/>
@@ -841,6 +846,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -848,14 +862,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B3E7EE6-44C7-4FC4-8FBC-FB4EDCF13A75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8092C04-3B86-48C3-AACA-8E92DC3775F3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -873,6 +879,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B3E7EE6-44C7-4FC4-8FBC-FB4EDCF13A75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF067616-7EC9-46F6-A8EA-7CB68C3B6A9D}">
   <ds:schemaRefs>

</xml_diff>